<commit_message>
Added arbeitspakete and vorlage-projektbeschreibung. completed added features in featurelist ToDo: add data to arbeitspakete & Featurelist
</commit_message>
<xml_diff>
--- a/doc/Featurelist.xlsx
+++ b/doc/Featurelist.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander Dietrich\Documents\Studium\1. Semester\Projekt\MultiPlay\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH\1_Semester\ITP-1\MultiPlay\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6048"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -170,10 +170,22 @@
     <t>Die Anzahl der aktiven Spieler pro Team wird angezeigt.</t>
   </si>
   <si>
-    <t>Nachdem für den Spielzug gevotet wurde, werden die Upvotes für den nächsten Zug im Spiel dargestellt.</t>
-  </si>
-  <si>
-    <t>Featureliste v.1.1</t>
+    <t>Arbeitspaket</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>z.B. 1</t>
+  </si>
+  <si>
+    <t>Nachdem für den Spielzug gevotet wurde, werden die Upvotes für den Zug im Spiel dargestellt.</t>
+  </si>
+  <si>
+    <t>Featureliste v.1.2</t>
+  </si>
+  <si>
+    <t>Design</t>
   </si>
 </sst>
 </file>
@@ -229,14 +241,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -554,25 +563,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="124.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="124.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>22</v>
@@ -584,7 +596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -612,8 +624,14 @@
       <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -638,8 +656,14 @@
       <c r="H3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -664,8 +688,11 @@
       <c r="H4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -690,8 +717,11 @@
       <c r="H5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -716,8 +746,11 @@
       <c r="H6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -742,8 +775,11 @@
       <c r="H7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -768,8 +804,11 @@
       <c r="H8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -794,8 +833,11 @@
       <c r="H9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -820,8 +862,11 @@
       <c r="H10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -846,8 +891,11 @@
       <c r="H11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -872,8 +920,11 @@
       <c r="H12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -889,8 +940,20 @@
       <c r="E13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -906,15 +969,27 @@
       <c r="E14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
         <v>30</v>
       </c>
       <c r="D15" t="s">
@@ -923,8 +998,20 @@
       <c r="E15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -940,13 +1027,25 @@
       <c r="E16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -957,13 +1056,25 @@
       <c r="E17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
         <v>37</v>
@@ -974,8 +1085,20 @@
       <c r="E18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -991,8 +1114,20 @@
       <c r="E19" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1008,8 +1143,20 @@
       <c r="E20" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1025,8 +1172,20 @@
       <c r="E21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1042,8 +1201,20 @@
       <c r="E22" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1059,8 +1230,20 @@
       <c r="E23" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1074,25 +1257,37 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
changed featurelists columns, changed name of Vorgage-Projektbeschreibung into Projektbeschreibung and added a lot of text to Projektbeschreibung
</commit_message>
<xml_diff>
--- a/doc/Featurelist.xlsx
+++ b/doc/Featurelist.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$I$2</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -41,9 +44,6 @@
     <t>Aufwand</t>
   </si>
   <si>
-    <t>Zuständig</t>
-  </si>
-  <si>
     <t>Startseite</t>
   </si>
   <si>
@@ -170,15 +170,9 @@
     <t>Die Anzahl der aktiven Spieler pro Team wird angezeigt.</t>
   </si>
   <si>
-    <t>Arbeitspaket</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>z.B. 1</t>
-  </si>
-  <si>
     <t>Nachdem für den Spielzug gevotet wurde, werden die Upvotes für den Zug im Spiel dargestellt.</t>
   </si>
   <si>
@@ -186,6 +180,9 @@
   </si>
   <si>
     <t>Design</t>
+  </si>
+  <si>
+    <t>Nicht begonnen</t>
   </si>
 </sst>
 </file>
@@ -563,7 +560,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
@@ -579,24 +576,24 @@
     <col min="6" max="6" width="8.6640625" customWidth="1"/>
     <col min="7" max="7" width="6.33203125" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -604,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
@@ -616,36 +613,30 @@
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -656,28 +647,25 @@
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="J3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -688,25 +676,25 @@
       <c r="H4">
         <v>10</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>8</v>
@@ -717,25 +705,25 @@
       <c r="H5">
         <v>10</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>8</v>
@@ -746,25 +734,25 @@
       <c r="H6">
         <v>10</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
       </c>
       <c r="F7">
         <v>8</v>
@@ -775,25 +763,25 @@
       <c r="H7">
         <v>10</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -804,25 +792,25 @@
       <c r="H8">
         <v>10</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -833,25 +821,25 @@
       <c r="H9">
         <v>10</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
         <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -862,25 +850,25 @@
       <c r="H10">
         <v>10</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -891,25 +879,25 @@
       <c r="H11">
         <v>10</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12">
         <v>2</v>
@@ -920,25 +908,25 @@
       <c r="H12">
         <v>10</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -949,25 +937,25 @@
       <c r="H13">
         <v>5</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -978,25 +966,25 @@
       <c r="H14">
         <v>8</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -1007,25 +995,25 @@
       <c r="H15">
         <v>10</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>34</v>
-      </c>
-      <c r="E16" t="s">
-        <v>35</v>
       </c>
       <c r="F16">
         <v>2</v>
@@ -1036,25 +1024,25 @@
       <c r="H16">
         <v>10</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1065,25 +1053,25 @@
       <c r="H17">
         <v>2</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
         <v>37</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>39</v>
       </c>
       <c r="F18">
         <v>3</v>
@@ -1094,25 +1082,25 @@
       <c r="H18">
         <v>10</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19">
         <v>3</v>
@@ -1123,25 +1111,25 @@
       <c r="H19">
         <v>8</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20">
         <v>6</v>
@@ -1152,25 +1140,25 @@
       <c r="H20">
         <v>10</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -1181,25 +1169,25 @@
       <c r="H21">
         <v>10</v>
       </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F22">
         <v>6</v>
@@ -1210,25 +1198,25 @@
       <c r="H22">
         <v>10</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23">
         <v>3</v>
@@ -1239,25 +1227,25 @@
       <c r="H23">
         <v>5</v>
       </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -1268,31 +1256,16 @@
       <c r="H24">
         <v>4</v>
       </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>26</v>
+      <c r="I24" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:I2">
+    <sortState ref="A3:I24">
+      <sortCondition ref="A2"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>